<commit_message>
bereit für ABS geprüft zu sein
</commit_message>
<xml_diff>
--- a/gant.xlsx
+++ b/gant.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lynx\Desktop\docu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72430483-0394-413A-89B5-66BDAD4E8597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736BF2F8-07EF-4BBB-8805-AB8823F218D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EF0892CD-E580-4ADF-A32B-AB44ACB1D7FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Лист1!$F$25</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Лист1!$F$25</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Лист1!$F$25</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Лист1!$F$25</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -129,6 +123,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-407]d\.\ mmm\.;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -154,12 +151,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -185,6 +176,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -203,13 +200,13 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -525,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799C22D8-D88E-4245-BED7-DF7300F6E53B}">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,247 +533,247 @@
     <col min="1" max="1" width="22.77734375" customWidth="1"/>
     <col min="2" max="2" width="49.5546875" customWidth="1"/>
     <col min="3" max="3" width="10.21875" customWidth="1"/>
-    <col min="4" max="17" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="16" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="7">
         <v>45201</v>
       </c>
-      <c r="D1" s="1">
-        <v>45202</v>
-      </c>
-      <c r="E1" s="1">
+      <c r="D1" s="7">
         <v>45203</v>
       </c>
-      <c r="F1" s="1">
+      <c r="E1" s="7">
         <v>45204</v>
       </c>
-      <c r="G1" s="1">
+      <c r="F1" s="7">
         <v>45205</v>
       </c>
-      <c r="H1" s="1">
+      <c r="G1" s="7">
         <v>45208</v>
       </c>
-      <c r="I1" s="1">
+      <c r="H1" s="7">
         <v>45209</v>
       </c>
-      <c r="J1" s="1">
+      <c r="I1" s="7">
         <v>45210</v>
       </c>
-      <c r="K1" s="1">
+      <c r="J1" s="7">
         <v>45211</v>
       </c>
-      <c r="L1" s="1">
+      <c r="K1" s="7">
         <v>45212</v>
       </c>
-      <c r="M1" s="1">
+      <c r="L1" s="7">
         <v>45215</v>
       </c>
-      <c r="N1" s="1">
+      <c r="M1" s="7">
         <v>45216</v>
       </c>
-      <c r="O1" s="1">
+      <c r="N1" s="7">
         <v>45217</v>
       </c>
-      <c r="P1" s="1">
+      <c r="O1" s="7">
         <v>45218</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="P1" s="7">
         <v>45219</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="4">
+      <c r="E11" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="5">
+      <c r="F13" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="5">
+      <c r="F14" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="5">
+      <c r="G15" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>18</v>
       </c>
-      <c r="I16" s="5">
+      <c r="H16" s="3">
         <v>8</v>
       </c>
-      <c r="J16" s="5">
+      <c r="I16" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="5">
+      <c r="I17" s="3">
         <v>6</v>
       </c>
-      <c r="K17" s="5">
+      <c r="J17" s="3">
         <v>6</v>
       </c>
-      <c r="L17" s="5">
+      <c r="K17" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="L18" s="5">
+      <c r="K18" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>23</v>
       </c>
-      <c r="M19" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L19" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>11</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
       </c>
-      <c r="N21" s="6">
+      <c r="M21" s="4">
         <v>2.5</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>12</v>
       </c>
       <c r="B23" t="s">
         <v>13</v>
       </c>
-      <c r="N23" s="7">
+      <c r="M23" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>14</v>
       </c>
-      <c r="N24" s="7">
+      <c r="M24" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>15</v>
       </c>
       <c r="B26" t="s">
         <v>16</v>
       </c>
-      <c r="O26" s="8">
+      <c r="N26" s="6">
         <v>5</v>
       </c>
-      <c r="P26" s="8">
+      <c r="O26" s="6">
         <v>5</v>
       </c>
-      <c r="Q26" s="8">
+      <c r="P26" s="6">
         <v>5</v>
       </c>
     </row>

</xml_diff>